<commit_message>
Cambios necesarios para inserción de los registros en base de datos
</commit_message>
<xml_diff>
--- a/app/src/main/assets/programme2.xlsx
+++ b/app/src/main/assets/programme2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Caperta personal\Universidad\EGC\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jupar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11145" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wednesday" sheetId="3" r:id="rId1"/>
@@ -209,12 +209,6 @@
     <t>Tools/Demos</t>
   </si>
   <si>
-    <t>TECHNICAL SESSIONS (F1.2)</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS (F2.2)</t>
-  </si>
-  <si>
     <t>9:15-10:15</t>
   </si>
   <si>
@@ -527,9 +521,6 @@
     <t>T1.2</t>
   </si>
   <si>
-    <t>DEMO SESSION (T2.1)</t>
-  </si>
-  <si>
     <t>Green PLE</t>
   </si>
   <si>
@@ -545,15 +536,9 @@
     <t>Demo session</t>
   </si>
   <si>
-    <t>20:00</t>
-  </si>
-  <si>
     <t>OPENING of the conference</t>
   </si>
   <si>
-    <t xml:space="preserve">KEYNOTE (W0.1) </t>
-  </si>
-  <si>
     <t>Keynote</t>
   </si>
   <si>
@@ -566,9 +551,6 @@
     <t>Marcello La Rosa</t>
   </si>
   <si>
-    <t xml:space="preserve">KEYNOTE (T0.1) </t>
-  </si>
-  <si>
     <t>T0.1</t>
   </si>
   <si>
@@ -611,43 +593,7 @@
     <t>50+10</t>
   </si>
   <si>
-    <t>TECHNICAL SESSIONS: Surveys and Reverse Engineering (F1.1)</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TECHNICAL SESSIONS parallel:  Configuration Mismatches (W1.1) </t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS parallel: Reverse Engineering (W2.1)</t>
-  </si>
-  <si>
-    <t>Test of time award talk (W3.1) Don Batory</t>
-  </si>
-  <si>
     <t>Awards +  Most influential paper awards talks</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS parallel (T1.2)</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS parallel: Implementing Product Lines (T1.1)</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS parallel: Service Product Lines (T3.1)</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS parallel: Testing Product Lines (T3.2)</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS: Implementing Product Lines 2 (F2.1)</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS parallel: GIS and Cyberphysical SPLs (W2.2)</t>
-  </si>
-  <si>
-    <t>TECHNICAL SESSIONS parallel: Modelbased Engineering SPLs (W1.2)</t>
   </si>
   <si>
     <t xml:space="preserve">Automated Repairing of Variability Models, An Empirical Study of Configuration Mismatches in Linux, Early Consistency Checking between Specification and Implementation Variabilities, Anomaly Detection and Explanation in Context-Aware Software Product Lines
@@ -707,10 +653,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Refactoring Java Software Product Lines, A Deep Dive into Android's Variability Realizations
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jongwook Kim, Don Batory and Danny Dig, Nicolas Fuberger, Bo Zhang and Martin Becker
 </t>
   </si>
@@ -727,6 +669,64 @@
   <si>
     <t xml:space="preserve">Jose Miguel Horcas Aguilera, Monica Pinto and Lidia Fuentes, David Wille, Kenny Wehling, Christoph Seidl, Martin Pluchator and Ina Schaefer, Yi Li, Chenguang Zhu, Julia Rubin and Marsha Chechik, Jabier Martinez, Wesley K. G. Assunsao and Tewfik Ziadi
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactoring Java Software Product Lines, A Deep Dive into Androids Variability Realizations
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(W0.1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(W1.1) </t>
+  </si>
+  <si>
+    <t>(W1.2)</t>
+  </si>
+  <si>
+    <t>(W2.1)</t>
+  </si>
+  <si>
+    <t>(W2.2)</t>
+  </si>
+  <si>
+    <t>(W3.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(T0.1) </t>
+  </si>
+  <si>
+    <t>(T1.1)</t>
+  </si>
+  <si>
+    <t>(T1.2)</t>
+  </si>
+  <si>
+    <t>(T2.1)</t>
+  </si>
+  <si>
+    <t>(T3.1)</t>
+  </si>
+  <si>
+    <t>(T3.2)</t>
+  </si>
+  <si>
+    <t>(F1.1)</t>
+  </si>
+  <si>
+    <t>(F1.2)</t>
+  </si>
+  <si>
+    <t>(F2.1)</t>
+  </si>
+  <si>
+    <t>(F2.2)</t>
+  </si>
+  <si>
+    <t>20:00-21:00</t>
+  </si>
+  <si>
+    <t>18:00-22:00</t>
   </si>
 </sst>
 </file>
@@ -1316,6 +1316,138 @@
   <dxfs count="33">
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="9"/>
         </patternFill>
@@ -1503,138 +1635,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1649,13 +1649,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Surname" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="email" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="session" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Surname" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="email" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="session" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1929,118 +1929,118 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.28515625" customWidth="1"/>
-    <col min="4" max="5" width="35.140625" customWidth="1"/>
+    <col min="2" max="3" width="45.33203125" customWidth="1"/>
+    <col min="4" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="35"/>
     </row>
-    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="36"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C3" s="40"/>
     </row>
-    <row r="4" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="C4" s="41"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="34"/>
     </row>
-    <row r="6" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="38"/>
     </row>
-    <row r="8" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>48</v>
-      </c>
       <c r="C9" s="34"/>
     </row>
-    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="C10" s="33"/>
     </row>
-    <row r="11" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C11" s="33"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2049,16 +2049,16 @@
       </c>
       <c r="C12" s="34"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>151</v>
+        <v>206</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="34"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
     </row>
   </sheetData>
@@ -2076,7 +2076,7 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="89" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="89" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2092,24 +2092,24 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.28515625" customWidth="1"/>
-    <col min="4" max="5" width="35.140625" customWidth="1"/>
+    <col min="2" max="3" width="45.33203125" customWidth="1"/>
+    <col min="4" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="35"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2118,54 +2118,54 @@
       </c>
       <c r="C2" s="42"/>
     </row>
-    <row r="3" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="C3" s="41"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="34"/>
     </row>
-    <row r="5" spans="1:3" ht="64.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="64.349999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C6" s="34"/>
     </row>
-    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>145</v>
+        <v>199</v>
       </c>
       <c r="C7" s="41"/>
     </row>
-    <row r="8" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2174,32 +2174,32 @@
       </c>
       <c r="C8" s="38"/>
     </row>
-    <row r="9" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="34"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="C10" s="34"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>53</v>
       </c>
       <c r="C11" s="34"/>
     </row>
@@ -2232,24 +2232,24 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="3" width="45.28515625" customWidth="1"/>
-    <col min="4" max="5" width="35.140625" customWidth="1"/>
+    <col min="2" max="3" width="45.33203125" customWidth="1"/>
+    <col min="4" max="5" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="35"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2258,18 +2258,18 @@
       </c>
       <c r="C2" s="42"/>
     </row>
-    <row r="3" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2278,18 +2278,18 @@
       </c>
       <c r="C4" s="34"/>
     </row>
-    <row r="5" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -2299,7 +2299,7 @@
       <c r="C6" s="44"/>
       <c r="D6" s="27"/>
     </row>
-    <row r="7" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="C7" s="44"/>
     </row>
-    <row r="8" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -2340,24 +2340,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="116.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="123.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="116.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="123.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -2371,10 +2371,10 @@
         <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>28</v>
@@ -2383,7 +2383,7 @@
         <v>29</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>30</v>
@@ -2395,7 +2395,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>23</v>
       </c>
@@ -2409,19 +2409,19 @@
         <v>23</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>34</v>
@@ -2433,7 +2433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>78</v>
       </c>
@@ -2447,16 +2447,16 @@
         <v>38</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
@@ -2469,7 +2469,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>15</v>
       </c>
@@ -2483,19 +2483,19 @@
         <v>36</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>37</v>
@@ -2507,7 +2507,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>22</v>
       </c>
@@ -2521,19 +2521,19 @@
         <v>23</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>37</v>
@@ -2545,7 +2545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -2559,19 +2559,19 @@
         <v>23</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>34</v>
@@ -2583,7 +2583,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -2597,19 +2597,19 @@
         <v>36</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>34</v>
@@ -2621,7 +2621,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>8</v>
       </c>
@@ -2635,19 +2635,19 @@
         <v>36</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>37</v>
@@ -2659,7 +2659,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>96</v>
       </c>
@@ -2673,19 +2673,19 @@
         <v>38</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>34</v>
@@ -2697,7 +2697,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>49</v>
       </c>
@@ -2711,19 +2711,19 @@
         <v>36</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>34</v>
@@ -2735,7 +2735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>25</v>
       </c>
@@ -2749,19 +2749,19 @@
         <v>36</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>34</v>
@@ -2773,7 +2773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>13</v>
       </c>
@@ -2787,19 +2787,19 @@
         <v>23</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>34</v>
@@ -2811,7 +2811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>108</v>
       </c>
@@ -2822,20 +2822,20 @@
         <v>35</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>34</v>
@@ -2844,10 +2844,10 @@
         <v>108</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>109</v>
       </c>
@@ -2858,20 +2858,20 @@
         <v>35</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>34</v>
@@ -2880,10 +2880,10 @@
         <v>109</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>110</v>
       </c>
@@ -2894,20 +2894,20 @@
         <v>35</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>34</v>
@@ -2916,19 +2916,19 @@
         <v>110</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2942,7 +2942,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2956,7 +2956,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2970,10 +2970,10 @@
       <c r="K27" s="7"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2987,7 +2987,7 @@
       <c r="K31" s="7"/>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="10"/>
       <c r="C32" s="8"/>
@@ -3001,7 +3001,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3015,7 +3015,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3029,7 +3029,7 @@
       <c r="K34" s="7"/>
       <c r="L34" s="8"/>
     </row>
-    <row r="35" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3043,20 +3043,20 @@
       <c r="K35" s="7"/>
       <c r="L35" s="8"/>
     </row>
-    <row r="36" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:12" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:L46" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <sortState ref="A2:L49">
@@ -3065,101 +3065,101 @@
   </autoFilter>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="B31:B33 B35 B27 B25 B2:B7 B11:B15">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="cellIs" dxfId="14" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"TP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3182,306 +3182,306 @@
       <selection activeCell="D4" sqref="C4:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="17"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="C18" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="18" t="s">
+      <c r="C20" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="B24" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="17"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="17"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="17"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="17"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="20" t="s">
+      <c r="C24" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="B25" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="C25" s="18" t="s">
         <v>115</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>117</v>
       </c>
       <c r="D25" s="17"/>
     </row>

</xml_diff>